<commit_message>
add colomn index to parsing excell
</commit_message>
<xml_diff>
--- a/bot.xlsx
+++ b/bot.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5">
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>nama</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
   <si>
     <t>6281392944603</t>
   </si>
@@ -970,19 +964,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="17.96875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -991,18 +985,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>